<commit_message>
[Updata] M-Fast Logo 삽입
</commit_message>
<xml_diff>
--- a/backbone/1. Backbone 성능.xlsx
+++ b/backbone/1. Backbone 성능.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1677029185" val="1062" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1677029185" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1677029185"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1677029185"/>
+      <pm:revision xmlns:pm="smNativeData" day="1679450610" val="1062" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1679450610" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1679450610" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1679450610"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
   <si>
     <t>Backbone</t>
   </si>
@@ -36,6 +36,9 @@
   <si>
     <t>FPS
 (avg 1000 iter)</t>
+  </si>
+  <si>
+    <t>Flops</t>
   </si>
   <si>
     <t>Params</t>
@@ -51,17 +54,21 @@
         <i val="0"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1677029185">
+            <pm:charSpec xmlns:pm="smNativeData" id="1679450610">
               <pm:latin face="Liberation Sans" sz="200" weight="bold" i="0"/>
-              <pm:cs weight="bold"/>
-              <pm:ea weight="bold"/>
-              <hyperlink type="3" url="mailto:acc@1" location="" text=""/>
+              <pm:cs/>
+              <pm:ea/>
             </pm:charSpec>
           </ext>
         </extLst>
       </rPr>
       <t>acc@1</t>
     </r>
+    <r>
+      <t xml:space="preserve"> (ImageNet1K)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Liberation Sans"/>
@@ -72,33 +79,10 @@
         <i val="0"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1677029185">
+            <pm:charSpec xmlns:pm="smNativeData" id="1679450610">
               <pm:latin face="Liberation Sans" sz="200" weight="bold" i="0"/>
-              <pm:cs weight="bold"/>
-              <pm:ea weight="bold"/>
-            </pm:charSpec>
-          </ext>
-        </extLst>
-      </rPr>
-      <t xml:space="preserve"> (ImageNet1K)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Liberation Sans"/>
-        <charset val="0"/>
-        <family val="2"/>
-        <sz val="10"/>
-        <b/>
-        <i val="0"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1677029185">
-              <pm:latin face="Liberation Sans" sz="200" weight="bold" i="0"/>
-              <pm:cs weight="bold"/>
-              <pm:ea weight="bold"/>
-              <hyperlink type="3" url="mailto:acc@5" location="" text=""/>
+              <pm:cs/>
+              <pm:ea/>
             </pm:charSpec>
           </ext>
         </extLst>
@@ -106,23 +90,6 @@
       <t>acc@5</t>
     </r>
     <r>
-      <rPr>
-        <rFont val="Liberation Sans"/>
-        <charset val="0"/>
-        <family val="2"/>
-        <sz val="10"/>
-        <b/>
-        <i val="0"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1677029185">
-              <pm:latin face="Liberation Sans" sz="200" weight="bold" i="0"/>
-              <pm:cs weight="bold"/>
-              <pm:ea weight="bold"/>
-            </pm:charSpec>
-          </ext>
-        </extLst>
-      </rPr>
       <t xml:space="preserve"> (ImageNet1K)</t>
     </r>
   </si>
@@ -263,24 +230,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <rFont val="Liberation Sans"/>
-        <charset val="0"/>
-        <family val="2"/>
-        <sz val="10"/>
-        <b val="0"/>
-        <i val="0"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1677029185">
-              <pm:latin face="Liberation Sans" sz="200" weight="normal" i="0"/>
-              <pm:cs/>
-              <pm:ea/>
-              <hyperlink type="6" url="https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet18.html" location="torchvision.models.resnet18" text=""/>
-            </pm:charSpec>
-          </ext>
-        </extLst>
-      </rPr>
       <t>https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet18.html#torchvision.models.resnet18</t>
     </r>
   </si>
@@ -304,24 +253,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <rFont val="Liberation Sans"/>
-        <charset val="0"/>
-        <family val="2"/>
-        <sz val="10"/>
-        <b val="0"/>
-        <i val="0"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1677029185">
-              <pm:latin face="Liberation Sans" sz="200" weight="normal" i="0"/>
-              <pm:cs/>
-              <pm:ea/>
-              <hyperlink type="6" url="https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet34.html" location="torchvision.models.resnet34" text=""/>
-            </pm:charSpec>
-          </ext>
-        </extLst>
-      </rPr>
       <t>https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet34.html#torchvision.models.resnet34</t>
     </r>
   </si>
@@ -387,24 +318,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <rFont val="Liberation Sans"/>
-        <charset val="0"/>
-        <family val="2"/>
-        <sz val="10"/>
-        <b val="0"/>
-        <i val="0"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1677029185">
-              <pm:latin face="Liberation Sans" sz="200" weight="normal" i="0"/>
-              <pm:cs/>
-              <pm:ea/>
-              <hyperlink type="6" url="https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet101.html" location="torchvision.models.resnet101" text=""/>
-            </pm:charSpec>
-          </ext>
-        </extLst>
-      </rPr>
       <t>https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet101.html#torchvision.models.resnet101</t>
     </r>
   </si>
@@ -428,24 +341,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <rFont val="Liberation Sans"/>
-        <charset val="0"/>
-        <family val="2"/>
-        <sz val="10"/>
-        <b val="0"/>
-        <i val="0"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1677029185">
-              <pm:latin face="Liberation Sans" sz="200" weight="normal" i="0"/>
-              <pm:cs/>
-              <pm:ea/>
-              <hyperlink type="6" url="https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet101.html" location="torchvision.models.resnet101" text=""/>
-            </pm:charSpec>
-          </ext>
-        </extLst>
-      </rPr>
       <t>https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet101.html#torchvision.models.resnet101</t>
     </r>
   </si>
@@ -779,7 +674,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₩&quot;_-;\-* #,##0.00\ &quot;₩&quot;_-;_-* &quot;-&quot;??\ &quot;₩&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₩_-;\-* #,##0.00\ _₩_-;_-* &quot;-&quot;??\ _₩_-;_-@_-"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="5">
     <font>
       <name val="Liberation Sans"/>
       <family val="2"/>
@@ -787,7 +682,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1677029185" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1679450610" ulstyle="none" kern="1">
             <pm:latin face="Liberation Sans" sz="200" lang="en-us"/>
             <pm:cs face="Lohit Devanagari" sz="200" lang="hi-in"/>
             <pm:ea face="Noto Sans CJK SC" sz="200" lang="zh-cn"/>
@@ -796,16 +691,16 @@
       </extLst>
     </font>
     <font>
-      <name val="Liberation Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1677029185" ulstyle="none" kern="1">
-            <pm:latin face="Liberation Sans" sz="200" lang="en-us"/>
-            <pm:cs face="Lohit Devanagari" sz="200" lang="hi-in"/>
-            <pm:ea face="Noto Sans CJK SC" sz="200" lang="zh-cn"/>
+          <pm:charSpec xmlns:pm="smNativeData" id="1679450610" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Times New Roman" sz="200" lang="default"/>
+            <pm:ea face="SimSun" sz="200" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -818,8 +713,23 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1677029185" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1679450610" ulstyle="none" kern="1">
             <pm:latin face="Liberation Sans" sz="200" lang="en-us" weight="bold"/>
+            <pm:cs face="Lohit Devanagari" sz="200" lang="hi-in" weight="bold"/>
+            <pm:ea face="Noto Sans CJK SC" sz="200" lang="zh-cn" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Liberation Sans"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1679450610" ulstyle="none" kern="1">
+            <pm:latin face="Liberation Sans" sz="200" lang="en-us"/>
             <pm:cs face="Lohit Devanagari" sz="200" lang="hi-in" weight="bold"/>
             <pm:ea face="Noto Sans CJK SC" sz="200" lang="zh-cn" weight="bold"/>
           </pm:charSpec>
@@ -834,90 +744,35 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1677029185" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1679450610" ulstyle="none" kern="1">
             <pm:latin face="Liberation Sans" sz="200" lang="en-us" weight="bold"/>
-            <pm:cs face="Lohit Devanagari" sz="200" lang="hi-in" weight="bold"/>
-            <pm:ea face="Noto Sans CJK SC" sz="200" lang="zh-cn" weight="bold"/>
-            <hyperlink type="3" url="mailto:acc@1" location="" text=""/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Liberation Sans"/>
-      <family val="2"/>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1677029185" ulstyle="none" kern="1">
-            <pm:latin face="Liberation Sans" sz="200" lang="en-us" weight="bold"/>
-            <pm:cs face="Lohit Devanagari" sz="200" lang="hi-in" weight="bold"/>
-            <pm:ea face="Noto Sans CJK SC" sz="200" lang="zh-cn" weight="bold"/>
-            <hyperlink type="3" url="mailto:acc@5" location="" text=""/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Liberation Sans"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1677029185" ulstyle="none" kern="1">
-            <pm:latin face="Liberation Sans" sz="200" lang="en-us"/>
             <pm:cs face="Lohit Devanagari" sz="200" lang="hi-in"/>
             <pm:ea face="Noto Sans CJK SC" sz="200" lang="zh-cn"/>
-            <hyperlink type="6" url="https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet18.html" location="torchvision.models.resnet18" text=""/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Liberation Sans"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1677029185" ulstyle="none" kern="1">
-            <pm:latin face="Liberation Sans" sz="200" lang="en-us"/>
-            <pm:cs face="Lohit Devanagari" sz="200" lang="hi-in"/>
-            <pm:ea face="Noto Sans CJK SC" sz="200" lang="zh-cn"/>
-            <hyperlink type="6" url="https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet34.html" location="torchvision.models.resnet34" text=""/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Liberation Sans"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1677029185" ulstyle="none" kern="1">
-            <pm:latin face="Liberation Sans" sz="200" lang="en-us"/>
-            <pm:cs face="Lohit Devanagari" sz="200" lang="hi-in"/>
-            <pm:ea face="Noto Sans CJK SC" sz="200" lang="zh-cn"/>
-            <hyperlink type="6" url="https://pytorch.org/vision/stable/models/generated/torchvision.models.resnet101.html" location="torchvision.models.resnet101" text=""/>
           </pm:charSpec>
         </ext>
       </extLst>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1679450610" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -933,7 +788,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1677029185"/>
+          <pm:border xmlns:pm="smNativeData" id="1679450610"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1679450610"/>
         </ext>
       </extLst>
     </border>
@@ -941,7 +815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -952,6 +826,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -959,10 +836,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1677029185" count="1">
-        <pm:charStyle name="보통" fontId="1" Id="1"/>
+      <pm:charStyles xmlns:pm="smNativeData" id="1679450610" count="1">
+        <pm:charStyle name="보통" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1677029185" count="10">
+      <pm:colors xmlns:pm="smNativeData" id="1679450610" count="10">
         <pm:color name="색: 24" rgb="FFFFCC"/>
         <pm:color name="색: 25" rgb="000E00"/>
         <pm:color name="색: 26" rgb="808080"/>
@@ -1235,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:AMJ28"/>
+  <dimension ref="A1:AMK28"/>
   <sheetViews>
     <sheetView tabSelected="1" colorId="22" defaultGridColor="0" view="normal" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1246,17 +1123,18 @@
     <col min="1" max="1" width="17.567568" customWidth="1" style="1"/>
     <col min="2" max="2" width="27.162162" customWidth="1" style="1"/>
     <col min="3" max="3" width="13.765766" customWidth="1" style="1"/>
-    <col min="4" max="4" width="13.531532" customWidth="1" style="1"/>
-    <col min="5" max="5" width="8.108108" customWidth="1" style="1"/>
-    <col min="6" max="7" width="19.234234" customWidth="1" style="1"/>
-    <col min="8" max="8" width="12.927928" customWidth="1" style="1"/>
-    <col min="9" max="9" width="34.486486" customWidth="1" style="1"/>
-    <col min="10" max="10" width="35.189189" customWidth="1" style="1"/>
-    <col min="11" max="1023" width="11.531532" customWidth="1" style="1"/>
-    <col min="1024" max="1024" width="11.531532" customWidth="1" style="0"/>
+    <col min="4" max="4" width="16.432432" customWidth="1" style="1"/>
+    <col min="5" max="5" width="5.612613" customWidth="1" style="1"/>
+    <col min="6" max="6" width="8.108108" customWidth="1" style="1"/>
+    <col min="7" max="8" width="19.234234" customWidth="1" style="1"/>
+    <col min="9" max="9" width="12.927928" customWidth="1" style="1"/>
+    <col min="10" max="10" width="34.486486" customWidth="1" style="1"/>
+    <col min="11" max="11" width="35.189189" customWidth="1" style="1"/>
+    <col min="12" max="1024" width="11.531532" customWidth="1" style="1"/>
+    <col min="1025" max="1025" width="11.531532" customWidth="1" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="29.85" customHeight="1">
+    <row r="1" spans="1:1025" ht="29.85" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1266,10 +1144,10 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1287,7 +1165,9 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -2300,34 +2180,32 @@
       <c r="AMG1" s="2"/>
       <c r="AMH1" s="2"/>
       <c r="AMI1" s="2"/>
-      <c r="AMJ1" s="3"/>
+      <c r="AMJ1" s="2"/>
+      <c r="AMK1" s="3"/>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>71.8780000000000001</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="H3" s="1" t="n">
         <v>90.2860000000000014</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -2335,28 +2213,28 @@
       <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>72.1539999999999964</v>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="n">
+        <v>72.1539999999999822</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>90.8220000000000027</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>23</v>
@@ -2364,28 +2242,28 @@
       <c r="J4" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="K4" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>74.0420000000000016</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="H5" s="1" t="n">
         <v>91.3400000000000034</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>30</v>
@@ -2393,28 +2271,28 @@
       <c r="J5" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="K5" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>75.2740000000000009</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="H6" s="1" t="n">
         <v>92.5660000000000025</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>37</v>
@@ -2422,28 +2300,28 @@
       <c r="J6" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="K6" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>67.6680000000000064</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="H7" s="1" t="n">
         <v>87.402000000000001</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>44</v>
@@ -2451,28 +2329,28 @@
       <c r="J7" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="K7" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="1" t="n">
         <v>69.7579999999999956</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="H8" s="1" t="n">
         <v>89.078000000000003</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>51</v>
@@ -2480,28 +2358,28 @@
       <c r="J8" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="K8" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>73.313999999999993</v>
+      <c r="F9" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="G9" s="1" t="n">
+        <v>73.3139999999999787</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>91.4200000000000017</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>58</v>
@@ -2509,28 +2387,28 @@
       <c r="J9" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="K9" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <v>76.1299999999999955</v>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="G10" s="1" t="n">
+        <v>76.1299999999999812</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>92.8619999999999948</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>65</v>
@@ -2538,28 +2416,28 @@
       <c r="J10" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="K10" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="1" t="n">
         <v>80.8580000000000041</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="H11" s="1" t="n">
         <v>95.4339999999999975</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>72</v>
@@ -2567,28 +2445,28 @@
       <c r="J11" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="K11" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>77.3739999999999952</v>
+      <c r="F12" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="G12" s="1" t="n">
+        <v>77.373999999999981</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>93.5460000000000065</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>79</v>
@@ -2596,28 +2474,28 @@
       <c r="J12" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="K12" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <v>81.8859999999999957</v>
+      <c r="F13" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="G13" s="1" t="n">
+        <v>81.8859999999999815</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>95.7800000000000011</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>86</v>
@@ -2625,28 +2503,28 @@
       <c r="J13" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="K13" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="1" t="n">
-        <v>78.3119999999999976</v>
+      <c r="F14" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="G14" s="1" t="n">
+        <v>78.3119999999999834</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>94.0460000000000065</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>93</v>
@@ -2654,28 +2532,28 @@
       <c r="J14" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="K14" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="1" t="n">
         <v>82.284000000000006</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="H15" s="1" t="n">
         <v>96.0019999999999953</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>100</v>
@@ -2683,28 +2561,28 @@
       <c r="J15" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="K15" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <v>77.617999999999995</v>
+      <c r="F16" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="G16" s="1" t="n">
+        <v>77.6179999999999808</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>93.6979999999999933</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>107</v>
@@ -2712,28 +2590,28 @@
       <c r="J16" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="K16" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="F17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="1" t="n">
         <v>81.1979999999999933</v>
       </c>
-      <c r="G17" s="1" t="n">
+      <c r="H17" s="1" t="n">
         <v>95.3400000000000034</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>114</v>
@@ -2741,28 +2619,28 @@
       <c r="J17" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="K17" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>79.3119999999999976</v>
+      <c r="F18" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="G18" s="1" t="n">
+        <v>79.3119999999999834</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>82.8340000000000032</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>121</v>
@@ -2770,28 +2648,28 @@
       <c r="J18" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="K18" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F19" s="1" t="n">
+      <c r="F19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" s="1" t="n">
         <v>94.5259999999999962</v>
       </c>
-      <c r="G19" s="1" t="n">
+      <c r="H19" s="1" t="n">
         <v>96.2279999999999944</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>128</v>
@@ -2799,28 +2677,28 @@
       <c r="J19" s="1" t="s">
         <v>129</v>
       </c>
+      <c r="K19" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="1" t="n">
-        <v>83.2459999999999951</v>
+      <c r="F20" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="G20" s="1" t="n">
+        <v>83.2459999999999809</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>96.4539999999999935</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>135</v>
@@ -2828,28 +2706,28 @@
       <c r="J20" s="1" t="s">
         <v>136</v>
       </c>
+      <c r="K20" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="F21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" s="1" t="n">
         <v>69.019999999999996</v>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="H21" s="1" t="n">
         <v>88.6280000000000001</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>142</v>
@@ -2857,28 +2735,28 @@
       <c r="J21" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="K21" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E22" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F22" s="1" t="n">
+      <c r="F22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G22" s="1" t="n">
         <v>70.3700000000000045</v>
       </c>
-      <c r="G22" s="1" t="n">
+      <c r="H22" s="1" t="n">
         <v>89.8100000000000023</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>149</v>
@@ -2886,28 +2764,28 @@
       <c r="J22" s="1" t="s">
         <v>150</v>
       </c>
+      <c r="K22" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E23" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F23" s="1" t="n">
+      <c r="F23" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G23" s="1" t="n">
         <v>69.9279999999999973</v>
       </c>
-      <c r="G23" s="1" t="n">
-        <v>89.2459999999999951</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>155</v>
+      <c r="H23" s="1" t="n">
+        <v>89.2459999999999809</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>156</v>
@@ -2915,28 +2793,28 @@
       <c r="J23" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="K23" s="1" t="s">
+        <v>158</v>
+      </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E24" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="1" t="n">
+      <c r="F24" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G24" s="1" t="n">
         <v>71.5859999999999985</v>
       </c>
-      <c r="G24" s="1" t="n">
+      <c r="H24" s="1" t="n">
         <v>90.3739999999999952</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>163</v>
@@ -2944,28 +2822,28 @@
       <c r="J24" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="K24" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F25" s="1" t="n">
+      <c r="F25" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G25" s="1" t="n">
         <v>71.5919999999999987</v>
       </c>
-      <c r="G25" s="1" t="n">
+      <c r="H25" s="1" t="n">
         <v>90.382000000000005</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>170</v>
@@ -2973,28 +2851,28 @@
       <c r="J25" s="1" t="s">
         <v>171</v>
       </c>
+      <c r="K25" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="F26" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G26" s="1" t="n">
         <v>73.3599999999999994</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="H26" s="1" t="n">
         <v>91.5160000000000053</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>177</v>
@@ -3002,28 +2880,28 @@
       <c r="J26" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="K26" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E27" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="F27" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G27" s="1" t="n">
         <v>72.3760000000000048</v>
       </c>
-      <c r="G27" s="1" t="n">
+      <c r="H27" s="1" t="n">
         <v>90.8760000000000048</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>184</v>
@@ -3031,41 +2909,44 @@
       <c r="J27" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="K27" s="1" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E28" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F28" s="1" t="n">
+      <c r="F28" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G28" s="1" t="n">
         <v>74.2180000000000035</v>
       </c>
-      <c r="G28" s="1" t="n">
+      <c r="H28" s="1" t="n">
         <v>91.8419999999999987</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>191</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>192</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1677029185" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1679450610" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3074,16 +2955,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1677029185" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1677029185" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1677029185" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1677029185" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1679450610" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1679450610" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1679450610" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1679450610" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1677029185" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1679450610" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>